<commit_message>
Correct problems with fixed interactions in Eduati network
</commit_message>
<xml_diff>
--- a/FALCON/ExampleDatasets/Eduati2017/Eduati_net2.xlsx
+++ b/FALCON/ExampleDatasets/Eduati2017/Eduati_net2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philippe.lucarelli\Documents\MATLAB\FALCON-dev\FALCON\ExampleDatasets\Eduati\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebastien.delandtshe\Documents\MATLAB\FALCON\FALCON\FALCON\ExampleDatasets\Eduati2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,17 +519,17 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D2" t="str">
         <f>A2&amp;B2&amp;C2</f>
-        <v>TGFb-&gt;TGFRb</v>
+        <v>EGF-&gt;EGFR</v>
       </c>
       <c r="E2" t="s">
         <v>37</v>
@@ -540,17 +540,17 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D44" si="0">A3&amp;B3&amp;C3</f>
-        <v>EGF-&gt;EGFR</v>
+        <f>A3&amp;B3&amp;C3</f>
+        <v>TGFb-&gt;TGFRb</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
@@ -570,7 +570,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D4:D44" si="0">A4&amp;B4&amp;C4</f>
         <v>HGF-&gt;PI3K</v>
       </c>
       <c r="E4" t="s">

</xml_diff>